<commit_message>
Update Snow Liwa app
</commit_message>
<xml_diff>
--- a/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
+++ b/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2091,6 +2091,358 @@
       </c>
       <c r="L36" t="inlineStr"/>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SL-20251204-001</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-12-04 00:48:53</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>fahaf</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0502992692</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>175</v>
+      </c>
+      <c r="G37" t="n">
+        <v>175</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>SL-20251204-002</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>2025-12-04 00:49:18</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>fahaf</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>0502992692</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>175</v>
+      </c>
+      <c r="G38" t="n">
+        <v>175</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>SL-20251204-003</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>2025-12-04 02:21:57</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>كل أيام الأسبوع</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>4:00pm - 12:00am</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
+        <v>175</v>
+      </c>
+      <c r="G39" t="n">
+        <v>175</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SL-20251204-004</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>2025-12-04 04:27:13</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>fahad</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>0502992932</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" t="n">
+        <v>175</v>
+      </c>
+      <c r="G40" t="n">
+        <v>175</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>SL-20251204-005</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>2025-12-04 04:27:13</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>fahad</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>0502992932</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" t="n">
+        <v>175</v>
+      </c>
+      <c r="G41" t="n">
+        <v>175</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SL-20251204-006</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>2025-12-04 05:03:20</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Fahad</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>0502992932</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" t="n">
+        <v>175</v>
+      </c>
+      <c r="G42" t="n">
+        <v>175</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SL-20251204-007</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>2025-12-04 05:04:26</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Fahad</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>0502992932</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" t="n">
+        <v>175</v>
+      </c>
+      <c r="G43" t="n">
+        <v>175</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>SL-20251204-008</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>2025-12-04 06:15:53</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>0502992932</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>175</v>
+      </c>
+      <c r="G44" t="n">
+        <v>175</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Hide sidebar on landing page; remove admin buttons; UI tweaks
</commit_message>
<xml_diff>
--- a/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
+++ b/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,214 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SL-20251205-001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-12-05 12:01:55</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>175</v>
+      </c>
+      <c r="G2" t="n">
+        <v>175</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>70db35eb-9a82-4522-bdae-3f705a8ac0a6</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>requires_payment_instrument</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://pay.ziina.com/payment_intent/70db35eb-9a82-4522-bdae-3f705a8ac0a6</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SL-20251205-002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-12-05 12:02:04</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>175</v>
+      </c>
+      <c r="G3" t="n">
+        <v>175</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3e0b0829-0a39-4f6a-b50d-799d1987355f</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>requires_payment_instrument</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://pay.ziina.com/payment_intent/3e0b0829-0a39-4f6a-b50d-799d1987355f</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>SL-20251205-003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-12-05 12:25:34</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>175</v>
+      </c>
+      <c r="G4" t="n">
+        <v>175</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>c65aa11b-2702-4d3b-b691-d0a2173d5350</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>requires_payment_instrument</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>https://pay.ziina.com/payment_intent/c65aa11b-2702-4d3b-b691-d0a2173d5350</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SL-20251205-004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-12-05 12:34:42</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fahad Ahmed </t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>175</v>
+      </c>
+      <c r="G5" t="n">
+        <v>175</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>ae5bcc5a-8027-4149-b15f-b746880a9c1a</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>requires_payment_instrument</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>https://pay.ziina.com/payment_intent/ae5bcc5a-8027-4149-b15f-b746880a9c1a</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update all ticket price mentions to 175 AED
</commit_message>
<xml_diff>
--- a/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
+++ b/Snow_Liwa1-main/snow_liwa/data/bookings.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2091,6 +2091,50 @@
       </c>
       <c r="L36" t="inlineStr"/>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SL-20251206-001</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>2025-12-06 20:06:27</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>fahaf</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
+        <v>175</v>
+      </c>
+      <c r="G37" t="n">
+        <v>175</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>